<commit_message>
Updated master.xml and removed 4 rows from testdata
</commit_message>
<xml_diff>
--- a/testData/SearchBusScheduleData.xlsx
+++ b/testData/SearchBusScheduleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huzaif\Documents\workspace\yatraJavaSelenium\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA5781A-C814-431C-A166-2B8195122701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7557C36D-7B04-4D47-892A-60FA258ABC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2715" yWindow="2475" windowWidth="16200" windowHeight="9983" xr2:uid="{A227A569-458B-49BE-9DC5-7990869442B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>BusFrom</t>
   </si>
@@ -53,27 +53,9 @@
     <t>Bangalore, Karnataka</t>
   </si>
   <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
     <t>Hyderabad</t>
   </si>
   <si>
-    <t>Bombay</t>
-  </si>
-  <si>
-    <t>Hubli</t>
-  </si>
-  <si>
-    <t>Dubai</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>BusFromShort</t>
   </si>
   <si>
@@ -84,15 +66,6 @@
   </si>
   <si>
     <t>Bangalore</t>
-  </si>
-  <si>
-    <t>Kolkata, West Bengal</t>
-  </si>
-  <si>
-    <t>Delhi, Delhi</t>
-  </si>
-  <si>
-    <t>Hubli, Karnataka</t>
   </si>
   <si>
     <t>DaysFromToday</t>
@@ -507,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72187BB4-BD79-4AE5-8232-323FF5559E36}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -524,30 +497,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -558,87 +531,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1">
         <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>